<commit_message>
Asignación de autores de recursos en greco matemáticas 7 tema 12
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion12/Escaleta_MA_07_12_CO (1).xlsx
+++ b/fuentes/contenidos/grado07/guion12/Escaleta_MA_07_12_CO (1).xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion12\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="215">
   <si>
     <t>Asignatura</t>
   </si>
@@ -396,12 +401,6 @@
     <t>Emplear imágenes con explicaciones sobre: razón entre segmentos, proporcion entre segmentos, segmentos proporcionales</t>
   </si>
   <si>
-    <t>Resolución de problemas de medidas empleando criterios de semejanza</t>
-  </si>
-  <si>
-    <t>Proyecto uso de homotecias para construir figuras a diferentes escalas</t>
-  </si>
-  <si>
     <t>Evaluación</t>
   </si>
   <si>
@@ -649,6 +648,27 @@
   </si>
   <si>
     <t>Practica con la semejanza de triángulos</t>
+  </si>
+  <si>
+    <t>Johanna Vera</t>
+  </si>
+  <si>
+    <t>Sandra Ortiz</t>
+  </si>
+  <si>
+    <t>Julian David</t>
+  </si>
+  <si>
+    <t>Jennifer Rojas</t>
+  </si>
+  <si>
+    <t>Resolución de problemas de medidas empleando criterios de semejanza. Construir en F13</t>
+  </si>
+  <si>
+    <t>Proyecto uso de homotecias para construir figuras a diferentes escalas. Construir en F13</t>
+  </si>
+  <si>
+    <t>Adriana Lasprilla</t>
   </si>
 </sst>
 </file>
@@ -1332,12 +1352,60 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1354,54 +1422,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1566,7 +1586,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1601,7 +1621,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1813,8 +1833,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:W96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="O94" sqref="O94:O95"/>
+    <sheetView tabSelected="1" topLeftCell="H6" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="H32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1832,107 +1852,107 @@
     <col min="11" max="11" width="13.28515625" style="44" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" style="44" customWidth="1"/>
     <col min="13" max="14" width="9.28515625" style="44" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" style="98" customWidth="1"/>
-    <col min="16" max="16" width="21" style="98" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" style="98" customWidth="1"/>
-    <col min="18" max="18" width="23" style="44" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" style="44" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.85546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" style="98" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="21" style="98" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" style="98" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="23" style="44" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" style="44" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="25.85546875" style="44" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="21.7109375" style="44" customWidth="1"/>
     <col min="22" max="16384" width="11.42578125" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="112" t="s">
+    <row r="1" spans="1:22" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="112" t="s">
+      <c r="D1" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="110" t="s">
+      <c r="E1" s="104" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="F1" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="114" t="s">
+      <c r="G1" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="108" t="s">
+      <c r="H1" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="108" t="s">
+      <c r="I1" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="118" t="s">
+      <c r="J1" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="116" t="s">
+      <c r="K1" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="114" t="s">
+      <c r="L1" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="120" t="s">
+      <c r="M1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="120"/>
-      <c r="O1" s="100" t="s">
+      <c r="N1" s="114"/>
+      <c r="O1" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="100" t="s">
+      <c r="P1" s="102" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="102" t="s">
+      <c r="Q1" s="118" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="106" t="s">
+      <c r="R1" s="122" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="102" t="s">
+      <c r="S1" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="104" t="s">
+      <c r="T1" s="120" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="102" t="s">
+      <c r="U1" s="118" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="113"/>
-      <c r="B2" s="111"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="115"/>
+    <row r="2" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="107"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="109"/>
       <c r="M2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="101"/>
-      <c r="P2" s="101"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="105"/>
-      <c r="U2" s="103"/>
-    </row>
-    <row r="3" spans="1:21" s="31" customFormat="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="119"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="119"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="119"/>
+    </row>
+    <row r="3" spans="1:22" s="31" customFormat="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>85</v>
       </c>
@@ -1957,7 +1977,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K3" s="25" t="s">
         <v>20</v>
@@ -1970,7 +1990,7 @@
       </c>
       <c r="N3" s="7"/>
       <c r="O3" s="27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P3" s="22" t="s">
         <v>20</v>
@@ -1990,8 +2010,11 @@
       <c r="U3" s="28" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V3" s="31" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>85</v>
       </c>
@@ -2009,7 +2032,7 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H4" s="22">
         <v>2</v>
@@ -2018,7 +2041,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K4" s="25" t="s">
         <v>20</v>
@@ -2031,7 +2054,7 @@
         <v>84</v>
       </c>
       <c r="O4" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P4" s="22" t="s">
         <v>19</v>
@@ -2046,13 +2069,16 @@
         <v>91</v>
       </c>
       <c r="T4" s="30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="U4" s="28" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V4" s="31" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>85</v>
       </c>
@@ -2111,7 +2137,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>85</v>
       </c>
@@ -2149,7 +2175,7 @@
         <v>39</v>
       </c>
       <c r="O6" s="38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="P6" s="39" t="s">
         <v>19</v>
@@ -2169,8 +2195,11 @@
       <c r="U6" s="40" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V6" s="31" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>85</v>
       </c>
@@ -2188,7 +2217,7 @@
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H7" s="22">
         <v>5</v>
@@ -2197,7 +2226,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="36" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K7" s="25" t="s">
         <v>19</v>
@@ -2208,13 +2237,13 @@
       <c r="M7" s="9"/>
       <c r="N7" s="8"/>
       <c r="O7" s="38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P7" s="39" t="s">
         <v>19</v>
       </c>
       <c r="Q7" s="40" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="R7" s="41" t="s">
         <v>90</v>
@@ -2223,13 +2252,13 @@
         <v>91</v>
       </c>
       <c r="T7" s="42" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="U7" s="40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="31" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="31" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>85</v>
       </c>
@@ -2245,7 +2274,7 @@
       <c r="E8" s="33"/>
       <c r="F8" s="34"/>
       <c r="G8" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H8" s="22">
         <v>6</v>
@@ -2254,7 +2283,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K8" s="25" t="s">
         <v>19</v>
@@ -2265,13 +2294,13 @@
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
       <c r="O8" s="38" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P8" s="39" t="s">
         <v>19</v>
       </c>
       <c r="Q8" s="40" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="R8" s="41" t="s">
         <v>87</v>
@@ -2280,13 +2309,13 @@
         <v>88</v>
       </c>
       <c r="T8" s="42" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="U8" s="40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>85</v>
       </c>
@@ -2302,7 +2331,7 @@
       <c r="E9" s="33"/>
       <c r="F9" s="34"/>
       <c r="G9" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H9" s="22">
         <v>7</v>
@@ -2311,7 +2340,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K9" s="25" t="s">
         <v>20</v>
@@ -2324,7 +2353,7 @@
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="P9" s="39" t="s">
         <v>20</v>
@@ -2336,16 +2365,19 @@
         <v>90</v>
       </c>
       <c r="S9" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="T9" s="42" t="s">
+        <v>200</v>
+      </c>
+      <c r="U9" s="40" t="s">
         <v>201</v>
       </c>
-      <c r="T9" s="42" t="s">
-        <v>202</v>
-      </c>
-      <c r="U9" s="40" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V9" s="31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>85</v>
       </c>
@@ -2361,7 +2393,7 @@
       <c r="E10" s="33"/>
       <c r="F10" s="34"/>
       <c r="G10" s="21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H10" s="22">
         <v>8</v>
@@ -2370,7 +2402,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="43" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K10" s="25" t="s">
         <v>19</v>
@@ -2381,7 +2413,7 @@
       <c r="M10" s="9"/>
       <c r="N10" s="8"/>
       <c r="O10" s="46" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P10" s="39" t="s">
         <v>19</v>
@@ -2390,19 +2422,19 @@
         <v>8</v>
       </c>
       <c r="R10" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="S10" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="S10" s="40" t="s">
-        <v>208</v>
-      </c>
       <c r="T10" s="42" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="U10" s="40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>85</v>
       </c>
@@ -2420,7 +2452,7 @@
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="47" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H11" s="22">
         <v>9</v>
@@ -2429,7 +2461,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="49" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K11" s="25" t="s">
         <v>19</v>
@@ -2440,7 +2472,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="46" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P11" s="39" t="s">
         <v>19</v>
@@ -2449,19 +2481,19 @@
         <v>5</v>
       </c>
       <c r="R11" s="41" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="S11" s="40" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="T11" s="42" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U11" s="40" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>85</v>
       </c>
@@ -2501,7 +2533,7 @@
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="P12" s="39" t="s">
         <v>19</v>
@@ -2516,13 +2548,16 @@
         <v>88</v>
       </c>
       <c r="T12" s="42" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="U12" s="40" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V12" s="31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>85</v>
       </c>
@@ -2562,7 +2597,7 @@
         <v>33</v>
       </c>
       <c r="O13" s="38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="P13" s="39" t="s">
         <v>19</v>
@@ -2577,13 +2612,16 @@
         <v>91</v>
       </c>
       <c r="T13" s="42" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="U13" s="40" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V13" s="31" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>85</v>
       </c>
@@ -2601,7 +2639,7 @@
       </c>
       <c r="F14" s="34"/>
       <c r="G14" s="21" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H14" s="22">
         <v>12</v>
@@ -2610,7 +2648,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="43" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K14" s="25" t="s">
         <v>19</v>
@@ -2621,7 +2659,7 @@
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P14" s="39" t="s">
         <v>19</v>
@@ -2630,19 +2668,19 @@
         <v>8</v>
       </c>
       <c r="R14" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="S14" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="S14" s="40" t="s">
-        <v>208</v>
-      </c>
       <c r="T14" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U14" s="40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>85</v>
       </c>
@@ -2656,13 +2694,13 @@
         <v>113</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H15" s="22">
         <v>13</v>
@@ -2671,7 +2709,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K15" s="25" t="s">
         <v>19</v>
@@ -2682,7 +2720,7 @@
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
       <c r="O15" s="38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P15" s="39" t="s">
         <v>19</v>
@@ -2691,19 +2729,19 @@
         <v>8</v>
       </c>
       <c r="R15" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="S15" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="S15" s="40" t="s">
-        <v>208</v>
-      </c>
       <c r="T15" s="42" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="U15" s="40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>85</v>
       </c>
@@ -2717,13 +2755,13 @@
         <v>113</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H16" s="22">
         <v>14</v>
@@ -2732,7 +2770,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="36" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K16" s="25" t="s">
         <v>19</v>
@@ -2743,7 +2781,7 @@
       <c r="M16" s="9"/>
       <c r="N16" s="8"/>
       <c r="O16" s="38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P16" s="39" t="s">
         <v>19</v>
@@ -2752,19 +2790,19 @@
         <v>8</v>
       </c>
       <c r="R16" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="S16" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="S16" s="40" t="s">
-        <v>208</v>
-      </c>
       <c r="T16" s="42" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="U16" s="40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>85</v>
       </c>
@@ -2778,13 +2816,13 @@
         <v>113</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H17" s="22">
         <v>15</v>
@@ -2793,7 +2831,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="43" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K17" s="25" t="s">
         <v>20</v>
@@ -2806,7 +2844,7 @@
       </c>
       <c r="N17" s="9"/>
       <c r="O17" s="38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="P17" s="39" t="s">
         <v>20</v>
@@ -2821,13 +2859,16 @@
         <v>88</v>
       </c>
       <c r="T17" s="42" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="U17" s="40" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V17" s="31" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>85</v>
       </c>
@@ -2841,13 +2882,13 @@
         <v>113</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H18" s="22">
         <v>16</v>
@@ -2856,7 +2897,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="43" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K18" s="25" t="s">
         <v>20</v>
@@ -2869,7 +2910,7 @@
         <v>33</v>
       </c>
       <c r="O18" s="38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="P18" s="39" t="s">
         <v>19</v>
@@ -2884,13 +2925,16 @@
         <v>91</v>
       </c>
       <c r="T18" s="42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="U18" s="40" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V18" s="31" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>85</v>
       </c>
@@ -2904,13 +2948,13 @@
         <v>113</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F19" s="34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H19" s="22">
         <v>17</v>
@@ -2932,7 +2976,7 @@
         <v>29</v>
       </c>
       <c r="O19" s="38" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="P19" s="39" t="s">
         <v>19</v>
@@ -2952,8 +2996,11 @@
       <c r="U19" s="40" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V19" s="31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>85</v>
       </c>
@@ -2967,13 +3014,13 @@
         <v>113</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H20" s="22">
         <v>18</v>
@@ -2982,7 +3029,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K20" s="25" t="s">
         <v>19</v>
@@ -2993,7 +3040,7 @@
       <c r="M20" s="8"/>
       <c r="N20" s="9"/>
       <c r="O20" s="38" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="P20" s="39" t="s">
         <v>19</v>
@@ -3002,19 +3049,19 @@
         <v>8</v>
       </c>
       <c r="R20" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="S20" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="S20" s="40" t="s">
-        <v>208</v>
-      </c>
       <c r="T20" s="42" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="U20" s="40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>85</v>
       </c>
@@ -3028,13 +3075,13 @@
         <v>113</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H21" s="22">
         <v>19</v>
@@ -3054,7 +3101,7 @@
       <c r="M21" s="8"/>
       <c r="N21" s="9"/>
       <c r="O21" s="38" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="P21" s="39" t="s">
         <v>19</v>
@@ -3063,19 +3110,19 @@
         <v>8</v>
       </c>
       <c r="R21" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="S21" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="S21" s="40" t="s">
-        <v>208</v>
-      </c>
       <c r="T21" s="42" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="U21" s="40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>85</v>
       </c>
@@ -3093,7 +3140,7 @@
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="21" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H22" s="22">
         <v>20</v>
@@ -3102,7 +3149,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K22" s="25" t="s">
         <v>20</v>
@@ -3115,7 +3162,7 @@
         <v>84</v>
       </c>
       <c r="O22" s="38" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="P22" s="39" t="s">
         <v>19</v>
@@ -3135,8 +3182,11 @@
       <c r="U22" s="40" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V22" s="31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>85</v>
       </c>
@@ -3150,7 +3200,7 @@
         <v>101</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="21" t="s">
@@ -3163,7 +3213,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K23" s="25" t="s">
         <v>19</v>
@@ -3174,7 +3224,7 @@
       <c r="M23" s="9"/>
       <c r="N23" s="8"/>
       <c r="O23" s="38" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="P23" s="39" t="s">
         <v>19</v>
@@ -3183,19 +3233,19 @@
         <v>8</v>
       </c>
       <c r="R23" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="S23" s="40" t="s">
         <v>206</v>
-      </c>
-      <c r="S23" s="40" t="s">
-        <v>208</v>
       </c>
       <c r="T23" s="42" t="s">
         <v>122</v>
       </c>
       <c r="U23" s="40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>85</v>
       </c>
@@ -3209,7 +3259,7 @@
         <v>101</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="21" t="s">
@@ -3222,7 +3272,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="43" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K24" s="25" t="s">
         <v>19</v>
@@ -3233,7 +3283,7 @@
       <c r="M24" s="9"/>
       <c r="N24" s="8"/>
       <c r="O24" s="38" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="P24" s="39" t="s">
         <v>19</v>
@@ -3242,19 +3292,19 @@
         <v>8</v>
       </c>
       <c r="R24" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="S24" s="40" t="s">
         <v>206</v>
-      </c>
-      <c r="S24" s="40" t="s">
-        <v>208</v>
       </c>
       <c r="T24" s="42" t="s">
         <v>121</v>
       </c>
       <c r="U24" s="40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" s="31" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" s="31" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>85</v>
       </c>
@@ -3268,11 +3318,11 @@
         <v>101</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H25" s="22">
         <v>23</v>
@@ -3294,7 +3344,7 @@
       </c>
       <c r="N25" s="9"/>
       <c r="O25" s="38" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="P25" s="39" t="s">
         <v>19</v>
@@ -3303,19 +3353,22 @@
         <v>8</v>
       </c>
       <c r="R25" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="S25" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="S25" s="40" t="s">
-        <v>208</v>
-      </c>
       <c r="T25" s="42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="U25" s="40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="V25" s="31" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>85</v>
       </c>
@@ -3329,11 +3382,11 @@
         <v>101</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H26" s="22">
         <v>24</v>
@@ -3342,7 +3395,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="43" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K26" s="25" t="s">
         <v>20</v>
@@ -3355,7 +3408,7 @@
         <v>33</v>
       </c>
       <c r="O26" s="38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="P26" s="39" t="s">
         <v>19</v>
@@ -3375,8 +3428,11 @@
       <c r="U26" s="40" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V26" s="31" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>85</v>
       </c>
@@ -3394,7 +3450,7 @@
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H27" s="22">
         <v>25</v>
@@ -3403,7 +3459,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K27" s="25" t="s">
         <v>19</v>
@@ -3416,7 +3472,7 @@
         <v>84</v>
       </c>
       <c r="O27" s="38" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="P27" s="39" t="s">
         <v>19</v>
@@ -3425,19 +3481,22 @@
         <v>8</v>
       </c>
       <c r="R27" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="S27" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="S27" s="40" t="s">
-        <v>208</v>
-      </c>
       <c r="T27" s="42" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="U27" s="40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="V27" s="31" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>85</v>
       </c>
@@ -3448,12 +3507,12 @@
         <v>114</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E28" s="33"/>
       <c r="F28" s="34"/>
       <c r="G28" s="21" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H28" s="22">
         <v>26</v>
@@ -3462,7 +3521,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="43" t="s">
-        <v>125</v>
+        <v>212</v>
       </c>
       <c r="K28" s="25" t="s">
         <v>20</v>
@@ -3495,8 +3554,11 @@
       <c r="U28" s="40" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V28" s="31" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>85</v>
       </c>
@@ -3507,12 +3569,12 @@
         <v>114</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E29" s="33"/>
       <c r="F29" s="34"/>
       <c r="G29" s="21" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H29" s="22">
         <v>27</v>
@@ -3521,7 +3583,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="43" t="s">
-        <v>126</v>
+        <v>213</v>
       </c>
       <c r="K29" s="25" t="s">
         <v>20</v>
@@ -3534,7 +3596,7 @@
         <v>83</v>
       </c>
       <c r="O29" s="38" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P29" s="39" t="s">
         <v>19</v>
@@ -3554,8 +3616,11 @@
       <c r="U29" s="40" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="V29" s="31" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>85</v>
       </c>
@@ -3566,7 +3631,7 @@
         <v>114</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E30" s="50"/>
       <c r="F30" s="34"/>
@@ -3580,7 +3645,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="43" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K30" s="25" t="s">
         <v>20</v>
@@ -3598,7 +3663,7 @@
       <c r="T30" s="52"/>
       <c r="U30" s="53"/>
     </row>
-    <row r="31" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>85</v>
       </c>
@@ -3609,12 +3674,12 @@
         <v>114</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E31" s="50"/>
       <c r="F31" s="34"/>
       <c r="G31" s="21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H31" s="22">
         <v>29</v>
@@ -3623,7 +3688,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="54" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K31" s="25" t="s">
         <v>19</v>
@@ -3649,13 +3714,13 @@
         <v>91</v>
       </c>
       <c r="T31" s="42" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="U31" s="40" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:21" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>85</v>
       </c>
@@ -3666,12 +3731,12 @@
         <v>114</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E32" s="50"/>
       <c r="F32" s="34"/>
       <c r="G32" s="21" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H32" s="22">
         <v>30</v>
@@ -3704,10 +3769,13 @@
         <v>91</v>
       </c>
       <c r="T32" s="42" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="U32" s="40" t="s">
         <v>92</v>
+      </c>
+      <c r="V32" s="31" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -4997,6 +5065,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5011,12 +5085,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A44">

</xml_diff>

<commit_message>
REVISIONES EN ENTORNO EDITORIAL: MA_07_12_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion12/Escaleta_MA_07_12_CO (1).xlsx
+++ b/fuentes/contenidos/grado07/guion12/Escaleta_MA_07_12_CO (1).xlsx
@@ -5,20 +5,21 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cen_3f_cdo_pc10a\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion12\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
     <sheet name="DATOS" sheetId="1" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$Q$1:$Q$86</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -599,9 +600,6 @@
     <t>Mapa conceptual sobre el tema La semejanza</t>
   </si>
   <si>
-    <t>Actividad sobre el concpeto de semejanza</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Las figuras semejantes</t>
   </si>
   <si>
@@ -669,6 +667,9 @@
   </si>
   <si>
     <t>Adriana Lasprilla</t>
+  </si>
+  <si>
+    <t>Actividad sobre el concepto de semejanza</t>
   </si>
 </sst>
 </file>
@@ -1352,18 +1353,36 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1404,24 +1423,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1833,8 +1834,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:W96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H6" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="H32" sqref="A32:XFD32"/>
+    <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="1155" topLeftCell="A3" activePane="bottomLeft"/>
+      <selection activeCell="H1" sqref="H1:I1048576"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1846,9 +1849,8 @@
     <col min="5" max="5" width="33.140625" style="96" customWidth="1"/>
     <col min="6" max="6" width="40.42578125" style="97" customWidth="1"/>
     <col min="7" max="7" width="66.28515625" style="44" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="98" customWidth="1"/>
-    <col min="9" max="9" width="11" style="98" customWidth="1"/>
-    <col min="10" max="10" width="59.28515625" style="44" customWidth="1"/>
+    <col min="8" max="9" width="0.5703125" style="98" customWidth="1"/>
+    <col min="10" max="10" width="83.5703125" style="44" customWidth="1"/>
     <col min="11" max="11" width="13.28515625" style="44" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" style="44" customWidth="1"/>
     <col min="13" max="14" width="9.28515625" style="44" customWidth="1"/>
@@ -1863,96 +1865,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="116" t="s">
+      <c r="C1" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="104" t="s">
+      <c r="E1" s="110" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="108" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="100" t="s">
+      <c r="H1" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="100" t="s">
+      <c r="I1" s="108" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="112" t="s">
+      <c r="J1" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="110" t="s">
+      <c r="K1" s="116" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="108" t="s">
+      <c r="L1" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="114" t="s">
+      <c r="M1" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="114"/>
-      <c r="O1" s="102" t="s">
+      <c r="N1" s="120"/>
+      <c r="O1" s="100" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="102" t="s">
+      <c r="P1" s="100" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="118" t="s">
+      <c r="Q1" s="102" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="122" t="s">
+      <c r="R1" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="118" t="s">
+      <c r="S1" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="120" t="s">
+      <c r="T1" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="118" t="s">
+      <c r="U1" s="102" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="107"/>
-      <c r="B2" s="105"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="109"/>
+      <c r="A2" s="113"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="115"/>
       <c r="M2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="119"/>
-      <c r="R2" s="123"/>
-      <c r="S2" s="119"/>
-      <c r="T2" s="121"/>
-      <c r="U2" s="119"/>
-    </row>
-    <row r="3" spans="1:22" s="31" customFormat="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="101"/>
+      <c r="P2" s="101"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="107"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="103"/>
+    </row>
+    <row r="3" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>85</v>
       </c>
@@ -2011,10 +2013,10 @@
         <v>89</v>
       </c>
       <c r="V3" s="31" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>85</v>
       </c>
@@ -2041,7 +2043,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
       <c r="K4" s="25" t="s">
         <v>20</v>
@@ -2069,16 +2071,16 @@
         <v>91</v>
       </c>
       <c r="T4" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="U4" s="28" t="s">
         <v>92</v>
       </c>
       <c r="V4" s="31" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" s="31" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>85</v>
       </c>
@@ -2137,7 +2139,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>85</v>
       </c>
@@ -2196,10 +2198,10 @@
         <v>92</v>
       </c>
       <c r="V6" s="31" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>85</v>
       </c>
@@ -2255,10 +2257,10 @@
         <v>134</v>
       </c>
       <c r="U7" s="40" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" s="31" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>85</v>
       </c>
@@ -2312,10 +2314,10 @@
         <v>136</v>
       </c>
       <c r="U8" s="40" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>85</v>
       </c>
@@ -2365,19 +2367,19 @@
         <v>90</v>
       </c>
       <c r="S9" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="T9" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="T9" s="42" t="s">
+      <c r="U9" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="U9" s="40" t="s">
-        <v>201</v>
-      </c>
       <c r="V9" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>85</v>
       </c>
@@ -2422,19 +2424,19 @@
         <v>8</v>
       </c>
       <c r="R10" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S10" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T10" s="42" t="s">
         <v>140</v>
       </c>
       <c r="U10" s="40" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>85</v>
       </c>
@@ -2481,19 +2483,19 @@
         <v>5</v>
       </c>
       <c r="R11" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="S11" s="40" t="s">
         <v>204</v>
-      </c>
-      <c r="S11" s="40" t="s">
-        <v>205</v>
       </c>
       <c r="T11" s="42" t="s">
         <v>141</v>
       </c>
       <c r="U11" s="40" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>85</v>
       </c>
@@ -2554,10 +2556,10 @@
         <v>89</v>
       </c>
       <c r="V12" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>85</v>
       </c>
@@ -2618,10 +2620,10 @@
         <v>92</v>
       </c>
       <c r="V13" s="31" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>85</v>
       </c>
@@ -2668,19 +2670,19 @@
         <v>8</v>
       </c>
       <c r="R14" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S14" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T14" s="42" t="s">
         <v>144</v>
       </c>
       <c r="U14" s="40" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>85</v>
       </c>
@@ -2729,19 +2731,19 @@
         <v>8</v>
       </c>
       <c r="R15" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S15" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="T15" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="T15" s="42" t="s">
-        <v>207</v>
-      </c>
       <c r="U15" s="40" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>85</v>
       </c>
@@ -2790,19 +2792,19 @@
         <v>8</v>
       </c>
       <c r="R16" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S16" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T16" s="42" t="s">
         <v>148</v>
       </c>
       <c r="U16" s="40" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>85</v>
       </c>
@@ -2865,10 +2867,10 @@
         <v>89</v>
       </c>
       <c r="V17" s="31" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>85</v>
       </c>
@@ -2931,10 +2933,10 @@
         <v>92</v>
       </c>
       <c r="V18" s="31" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>85</v>
       </c>
@@ -2997,10 +2999,10 @@
         <v>92</v>
       </c>
       <c r="V19" s="31" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>85</v>
       </c>
@@ -3049,19 +3051,19 @@
         <v>8</v>
       </c>
       <c r="R20" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S20" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T20" s="42" t="s">
         <v>155</v>
       </c>
       <c r="U20" s="40" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>85</v>
       </c>
@@ -3110,19 +3112,19 @@
         <v>8</v>
       </c>
       <c r="R21" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S21" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T21" s="42" t="s">
         <v>157</v>
       </c>
       <c r="U21" s="40" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>85</v>
       </c>
@@ -3140,7 +3142,7 @@
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H22" s="22">
         <v>20</v>
@@ -3149,7 +3151,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="36" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K22" s="25" t="s">
         <v>20</v>
@@ -3183,10 +3185,10 @@
         <v>92</v>
       </c>
       <c r="V22" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>85</v>
       </c>
@@ -3233,19 +3235,19 @@
         <v>8</v>
       </c>
       <c r="R23" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S23" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T23" s="42" t="s">
         <v>122</v>
       </c>
       <c r="U23" s="40" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>85</v>
       </c>
@@ -3292,19 +3294,19 @@
         <v>8</v>
       </c>
       <c r="R24" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S24" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T24" s="42" t="s">
         <v>121</v>
       </c>
       <c r="U24" s="40" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" s="31" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>85</v>
       </c>
@@ -3353,22 +3355,22 @@
         <v>8</v>
       </c>
       <c r="R25" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S25" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T25" s="42" t="s">
         <v>160</v>
       </c>
       <c r="U25" s="40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="V25" s="31" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>85</v>
       </c>
@@ -3429,10 +3431,10 @@
         <v>92</v>
       </c>
       <c r="V26" s="31" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>85</v>
       </c>
@@ -3481,22 +3483,22 @@
         <v>8</v>
       </c>
       <c r="R27" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S27" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T27" s="42" t="s">
         <v>162</v>
       </c>
       <c r="U27" s="40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="V27" s="31" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>85</v>
       </c>
@@ -3512,7 +3514,7 @@
       <c r="E28" s="33"/>
       <c r="F28" s="34"/>
       <c r="G28" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H28" s="22">
         <v>26</v>
@@ -3521,7 +3523,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K28" s="25" t="s">
         <v>20</v>
@@ -3555,10 +3557,10 @@
         <v>92</v>
       </c>
       <c r="V28" s="31" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>85</v>
       </c>
@@ -3574,7 +3576,7 @@
       <c r="E29" s="33"/>
       <c r="F29" s="34"/>
       <c r="G29" s="21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H29" s="22">
         <v>27</v>
@@ -3583,7 +3585,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K29" s="25" t="s">
         <v>20</v>
@@ -3617,10 +3619,10 @@
         <v>92</v>
       </c>
       <c r="V29" s="31" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>85</v>
       </c>
@@ -3663,7 +3665,7 @@
       <c r="T30" s="52"/>
       <c r="U30" s="53"/>
     </row>
-    <row r="31" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>85</v>
       </c>
@@ -3714,13 +3716,13 @@
         <v>91</v>
       </c>
       <c r="T31" s="42" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="U31" s="40" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:22" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>85</v>
       </c>
@@ -3769,13 +3771,13 @@
         <v>91</v>
       </c>
       <c r="T32" s="42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="U32" s="40" t="s">
         <v>92</v>
       </c>
       <c r="V32" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -5065,12 +5067,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5085,6 +5081,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A44">
@@ -7092,4 +7094,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>70</v>
+      </c>
+      <c r="D3">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <f>C3*D4</f>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <f>C4*D3</f>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f>C3/C4</f>
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f>D3/D4</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>